<commit_message>
add new testing error to testing section and document
</commit_message>
<xml_diff>
--- a/testing/testing.xlsx
+++ b/testing/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c2d4706cdffd893/3. EDUCATION/FULLSTACK SOFTWARE DEVELOPMENT DIPLOMA/MS-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="337" documentId="8_{67B22251-1CDE-4A42-BE5A-D1762AAEA8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1859D88C-4B81-46FB-AC2F-6D213D3F7363}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="8_{67B22251-1CDE-4A42-BE5A-D1762AAEA8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C71C5A2-919C-4328-988E-C591535A7E31}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="210">
   <si>
     <t>Comments/Fixes</t>
   </si>
@@ -671,6 +671,18 @@
   </si>
   <si>
     <t>1. Check nav bar for links to either of these features they should not be visible</t>
+  </si>
+  <si>
+    <t>all errors in django auto generated files</t>
+  </si>
+  <si>
+    <t>all files and code auto generated by django and causing errors were not refactored</t>
+  </si>
+  <si>
+    <t>avoid using null=true</t>
+  </si>
+  <si>
+    <t>This is an informative message and not an error or warning so was left alone. An attempt was made to remove it and then change the migrations but resulted in having to reset all migrations and repopulate the database in gitpod environment to rectify the issues caused be trying to change the model after the postgres database had been created . On the advice of my mentor as it is only a blue informative message we have decided to leave it as is for now but for future projects the structure of a a model such as this would not include it especially on items such as sku which are usually requierd fields in ecommerce.</t>
   </si>
 </sst>
 </file>
@@ -975,24 +987,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1005,6 +1017,36 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1012,36 +1054,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1405,11 +1417,11 @@
         <v>68</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
@@ -1420,11 +1432,11 @@
         <v>12</v>
       </c>
       <c r="C4" s="13"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="14" t="s">
         <v>121</v>
       </c>
@@ -1434,11 +1446,11 @@
         <v>13</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>121</v>
       </c>
@@ -1448,11 +1460,11 @@
         <v>14</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="14" t="s">
         <v>121</v>
       </c>
@@ -1462,11 +1474,11 @@
         <v>16</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="14" t="s">
         <v>121</v>
       </c>
@@ -1476,11 +1488,11 @@
         <v>18</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="14" t="s">
         <v>121</v>
       </c>
@@ -1490,11 +1502,11 @@
         <v>135</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="14" t="s">
         <v>121</v>
       </c>
@@ -1504,11 +1516,11 @@
         <v>181</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="14" t="s">
         <v>121</v>
       </c>
@@ -1518,11 +1530,11 @@
         <v>69</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="14" t="s">
         <v>121</v>
       </c>
@@ -1532,11 +1544,11 @@
         <v>137</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="46"/>
       <c r="G12" s="14" t="s">
         <v>121</v>
       </c>
@@ -1546,11 +1558,11 @@
         <v>20</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="2:15" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1558,11 +1570,11 @@
         <v>47</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
       <c r="G14" s="15" t="s">
         <v>121</v>
       </c>
@@ -1572,11 +1584,11 @@
         <v>122</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="15" t="s">
         <v>121</v>
       </c>
@@ -1586,11 +1598,11 @@
         <v>72</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="15" t="s">
         <v>121</v>
       </c>
@@ -1600,11 +1612,11 @@
         <v>74</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="46"/>
       <c r="G17" s="15" t="s">
         <v>121</v>
       </c>
@@ -1614,11 +1626,11 @@
         <v>123</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
       <c r="G18" s="15" t="s">
         <v>121</v>
       </c>
@@ -1628,11 +1640,11 @@
         <v>49</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="15" t="s">
         <v>121</v>
       </c>
@@ -1642,11 +1654,11 @@
         <v>76</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="46"/>
       <c r="G20" s="15" t="s">
         <v>121</v>
       </c>
@@ -1656,11 +1668,11 @@
         <v>139</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="15" t="s">
         <v>121</v>
       </c>
@@ -1670,9 +1682,9 @@
         <v>22</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1680,11 +1692,11 @@
         <v>141</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="15" t="s">
         <v>121</v>
       </c>
@@ -1694,11 +1706,11 @@
         <v>142</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="14" t="s">
         <v>143</v>
       </c>
@@ -1708,11 +1720,11 @@
         <v>53</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="15" t="s">
         <v>121</v>
       </c>
@@ -1722,11 +1734,11 @@
         <v>144</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="15" t="s">
         <v>121</v>
       </c>
@@ -1736,23 +1748,24 @@
         <v>56</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="15" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D12:F12"/>
@@ -1766,13 +1779,12 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1823,11 +1835,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1838,11 +1850,11 @@
         <v>23</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="10" t="s">
         <v>121</v>
       </c>
@@ -1852,11 +1864,11 @@
         <v>146</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="10" t="s">
         <v>148</v>
       </c>
@@ -1866,11 +1878,11 @@
         <v>186</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="10" t="s">
         <v>121</v>
       </c>
@@ -1936,11 +1948,11 @@
         <v>155</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="10" t="s">
         <v>121</v>
       </c>
@@ -2053,24 +2065,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2114,11 +2126,11 @@
       <c r="D3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
       <c r="H3" s="21" t="s">
         <v>33</v>
       </c>
@@ -2129,9 +2141,9 @@
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="21"/>
     </row>
     <row r="5" spans="2:8" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2142,11 +2154,11 @@
       <c r="D5" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="14" t="s">
         <v>121</v>
       </c>
@@ -2159,11 +2171,11 @@
       <c r="D6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="14" t="s">
         <v>121</v>
       </c>
@@ -2210,11 +2222,11 @@
       <c r="D9" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="36" t="s">
         <v>121</v>
       </c>
@@ -2224,11 +2236,11 @@
         <v>38</v>
       </c>
       <c r="C10" s="29"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53"/>
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
@@ -2255,11 +2267,11 @@
       <c r="D12" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="18" t="s">
         <v>121</v>
       </c>
@@ -2286,11 +2298,11 @@
         <v>39</v>
       </c>
       <c r="C14" s="29"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
     </row>
     <row r="15" spans="2:8" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
@@ -2317,11 +2329,11 @@
       <c r="D16" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="18" t="s">
         <v>121</v>
       </c>
@@ -2348,11 +2360,11 @@
         <v>40</v>
       </c>
       <c r="C18" s="29"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="59"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
     </row>
     <row r="19" spans="2:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
@@ -2376,11 +2388,11 @@
         <v>41</v>
       </c>
       <c r="C20" s="29"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="59"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
     </row>
     <row r="21" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="38" t="s">
@@ -2404,11 +2416,11 @@
         <v>42</v>
       </c>
       <c r="C22" s="29"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="59"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="2:8" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
@@ -2435,11 +2447,11 @@
       <c r="D24" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="40" t="s">
         <v>121</v>
       </c>
@@ -2480,16 +2492,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="E8:G8"/>
@@ -2505,6 +2507,16 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="D14:H14"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="E19:G19"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2515,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FACEED-12E5-4B7A-B200-FE4D145D4ADD}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,11 +2560,11 @@
         <v>5</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
       <c r="H3" s="16" t="s">
         <v>7</v>
       </c>
@@ -2565,11 +2577,11 @@
         <v>85</v>
       </c>
       <c r="D4" s="13"/>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="14" t="s">
         <v>86</v>
       </c>
@@ -2582,11 +2594,11 @@
         <v>80</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="14" t="s">
         <v>83</v>
       </c>
@@ -2599,11 +2611,11 @@
         <v>119</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="14" t="s">
         <v>120</v>
       </c>
@@ -2616,11 +2628,11 @@
         <v>95</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="18" t="s">
         <v>97</v>
       </c>
@@ -2633,11 +2645,11 @@
         <v>102</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="18" t="s">
         <v>104</v>
       </c>
@@ -2650,11 +2662,11 @@
         <v>105</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="18" t="s">
         <v>108</v>
       </c>
@@ -2667,11 +2679,11 @@
         <v>110</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="18" t="s">
         <v>112</v>
       </c>
@@ -2684,11 +2696,11 @@
         <v>117</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
       <c r="H11" s="18" t="s">
         <v>118</v>
       </c>
@@ -2701,11 +2713,11 @@
         <v>114</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="53"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
       <c r="H12" s="18" t="s">
         <v>115</v>
       </c>
@@ -2718,33 +2730,33 @@
         <v>128</v>
       </c>
       <c r="D13" s="35"/>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="53"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="63"/>
       <c r="H13" s="36" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="17"/>
       <c r="E15" s="50" t="s">
         <v>89</v>
@@ -2756,16 +2768,16 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="18" t="s">
         <v>100</v>
       </c>
@@ -2776,20 +2788,20 @@
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="18" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="17"/>
       <c r="E18" s="50" t="s">
         <v>93</v>
@@ -2801,127 +2813,149 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20" spans="2:10" s="37" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="43"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="59"/>
     </row>
     <row r="21" spans="2:10" s="37" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="59"/>
     </row>
     <row r="22" spans="2:10" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="43"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="17"/>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="46"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="2:10" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="C24" s="43"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="41" t="s">
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="59"/>
+    </row>
+    <row r="25" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="43"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="60" t="s">
         <v>198</v>
       </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41" t="s">
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
+    </row>
+    <row r="26" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="43"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="60" t="s">
         <v>200</v>
       </c>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="59"/>
     </row>
     <row r="27" spans="2:10" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="43"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="59"/>
       <c r="J27" s="37"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="46"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
       <c r="J28" s="37"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="46"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="59"/>
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -2931,32 +2965,11 @@
       <c r="J31" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
+  <mergeCells count="43">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="E29:H29"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="B2:H2"/>
@@ -2971,6 +2984,31 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>